<commit_message>
CDR by logistic function based on CDR 1990-2012 estimates, not on annual WHO estimates
Output % reactivation vs new infections, and number of ppl newly infected

mort drop to change at 2000 and 2010, fertdrop to change at 1990.
</commit_message>
<xml_diff>
--- a/Vaccine duration modelling_RCH.xlsx
+++ b/Vaccine duration modelling_RCH.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="220" windowWidth="25360" windowHeight="15840" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="6720" yWindow="100" windowWidth="25360" windowHeight="15840" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="5yr" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2094" uniqueCount="23">
   <si>
     <t>Adolescent/Adult vaccine</t>
   </si>
@@ -276,8 +276,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="79">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -403,7 +405,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="79">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -443,6 +445,7 @@
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -482,6 +485,7 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6853,8 +6857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="AH7" sqref="AH7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8519,7 +8523,9 @@
       <c r="W26" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="X26" s="26"/>
+      <c r="X26" s="27" t="s">
+        <v>5</v>
+      </c>
       <c r="Y26" s="26"/>
       <c r="Z26" s="26"/>
       <c r="AA26" s="26"/>

</xml_diff>